<commit_message>
From bjo-sea01 fix long- 2023-12-01.014416
</commit_message>
<xml_diff>
--- a/config/config/track-and-trace.SEA01.xlsx
+++ b/config/config/track-and-trace.SEA01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leogzl/Documents/01. Work/java/src.client/YSH.Client/client/FSY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Documents/docker/data/client/ysh/client/bjo-sea01/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6725F4F5-61E7-9643-AAC1-407AF395B83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F68DC4-BE8B-2747-9828-EFA8F05B3B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="3440" windowWidth="25220" windowHeight="18620" activeTab="2" xr2:uid="{D1E400A9-94D3-C340-ADBB-65EA67C8B266}"/>
+    <workbookView xWindow="6760" yWindow="3440" windowWidth="25220" windowHeight="18620" xr2:uid="{D1E400A9-94D3-C340-ADBB-65EA67C8B266}"/>
   </bookViews>
   <sheets>
     <sheet name="FISH-DISPATCH" sheetId="1" r:id="rId1"/>
@@ -71,12 +71,6 @@
     <t>batchNumber</t>
   </si>
   <si>
-    <t>GOODS_RECEIPT</t>
-  </si>
-  <si>
-    <t>GOODS_ISSUE</t>
-  </si>
-  <si>
     <t>INVOICE</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>customer</t>
   </si>
   <si>
-    <t>CUSTOMER_SALES</t>
-  </si>
-  <si>
     <t>Business Transaction</t>
   </si>
   <si>
@@ -150,6 +141,15 @@
   </si>
   <si>
     <t>freezing</t>
+  </si>
+  <si>
+    <t>GOODS-RECEIPT</t>
+  </si>
+  <si>
+    <t>GOODS-ISSUE</t>
+  </si>
+  <si>
+    <t>CUSTOMER-SALES</t>
   </si>
 </sst>
 </file>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04ED85E3-57D6-5B44-8F00-3277DA2B83C8}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,19 +529,19 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -563,13 +563,13 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -583,19 +583,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -609,19 +609,19 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -635,19 +635,19 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -665,7 +665,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,97 +682,97 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F21B3C9-FF90-7F4B-8AB8-6FC94D23185E}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,68 +807,68 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>